<commit_message>
thesis changes. metric space ode theory complete. BBM complete
</commit_message>
<xml_diff>
--- a/teaching/10550/section-2/10550-2.xlsx
+++ b/teaching/10550/section-2/10550-2.xlsx
@@ -386,12 +386,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -755,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65:J70"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2558,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -2651,10 +2645,10 @@
         <v>49</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I51">
         <v>4</v>
@@ -3272,10 +3266,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>